<commit_message>
add table of company name and url from RAEX
</commit_message>
<xml_diff>
--- a/RAEX list.xlsx
+++ b/RAEX list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Кирилл\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demonveen/Downloads/ESG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0D7883-4213-44C7-B160-776A2E669ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD4518A-BBE6-244D-960F-ED1A2D4FDED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{235FC77D-80C7-224E-9415-310BA195EF61}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="26660" xr2:uid="{235FC77D-80C7-224E-9415-310BA195EF61}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -2226,24 +2226,24 @@
       <selection pane="bottomRight" activeCell="N164" sqref="N164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.296875" customWidth="1"/>
-    <col min="14" max="14" width="156.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.33203125" customWidth="1"/>
+    <col min="14" max="14" width="156.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>294</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -5745,7 +5745,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -6308,7 +6308,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -6745,7 +6745,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -8129,7 +8129,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -8953,7 +8953,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -8991,7 +8991,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -9079,7 +9079,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>285</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>285</v>
       </c>
@@ -9208,7 +9208,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>285</v>
       </c>

</xml_diff>